<commit_message>
añadiendo requisitos de viaje pasajero
</commit_message>
<xml_diff>
--- a/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
+++ b/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Documentos\GitHub\ElmerX\Desarrollo\STSM\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diaz\Documents\gestion\ElmerX\Desarrollo\STSM\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893500FA-08ED-4DF4-A705-700D4AE98902}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -54,13 +55,64 @@
   </si>
   <si>
     <t xml:space="preserve">Prototipo </t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>VIAJE</t>
+  </si>
+  <si>
+    <t>Pasajero</t>
+  </si>
+  <si>
+    <t>Buscar viaje</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir el ingreso de palabras clave, para la busqueda de viajes, donde debe mostrar las coincidencias con los viajes que tienen aun cupos disponibles.</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir solicitar un cupo en el viaje que selecciono el pasajero.</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Rechazar cupo</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir rechazar un cupo del viaje en el que se encuentra en el pasajero.</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ver la información del viaje: la ruta, numero de asientos disponibles, información del automovil (placa, modelo, etc).</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ver la información del conductor: su nombre, la escuela a la que pertenece, edad, numero de telefono.</t>
+  </si>
+  <si>
+    <t>solicitar cupo</t>
+  </si>
+  <si>
+    <t>Ver información del viaje</t>
+  </si>
+  <si>
+    <t>Ver información del conductor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -82,13 +134,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -316,10 +361,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -346,17 +391,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -365,7 +409,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,20 +418,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -412,6 +456,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,7 +498,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -537,6 +590,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -572,6 +642,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -747,11 +834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -765,13 +852,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -783,61 +870,111 @@
     </row>
     <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
+      <c r="B8" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -845,7 +982,7 @@
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -853,7 +990,7 @@
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -861,7 +998,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -869,7 +1006,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
@@ -877,7 +1014,7 @@
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -885,7 +1022,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -893,7 +1030,7 @@
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
@@ -901,7 +1038,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -909,7 +1046,7 @@
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -917,7 +1054,7 @@
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -925,7 +1062,7 @@
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="15"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -933,7 +1070,7 @@
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -941,7 +1078,7 @@
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="15"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -949,7 +1086,7 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -957,19 +1094,20 @@
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:F3"/>
+  <autoFilter ref="B3:F3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -981,11 +1119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1002,14 +1140,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1024,63 +1162,63 @@
     </row>
     <row r="3" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="5"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="31"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="32"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="33"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1089,9 +1227,9 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1100,9 +1238,9 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1111,9 +1249,9 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1123,41 +1261,41 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1168,7 +1306,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -1179,7 +1317,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -1190,7 +1328,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1201,7 +1339,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1212,7 +1350,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1223,7 +1361,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1234,7 +1372,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1245,7 +1383,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="19"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1256,7 +1394,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1267,7 +1405,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Cronograma actualizado y Requisitos Agregados-Steve
</commit_message>
<xml_diff>
--- a/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
+++ b/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -54,13 +54,67 @@
   </si>
   <si>
     <t xml:space="preserve">Prototipo </t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>RECLAMOS</t>
+  </si>
+  <si>
+    <t>Pasajero</t>
+  </si>
+  <si>
+    <t>Enviar Reclamo</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ingresar un nuevo reclamo sobre el viaje realizado.</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Sistema</t>
+  </si>
+  <si>
+    <t>Sancionar conductor</t>
+  </si>
+  <si>
+    <t>El sistema sancionara al conductor al confirmar si el reclamo hecho es valido.</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Enviar notificacion de reclamo</t>
+  </si>
+  <si>
+    <t>El sistema enviara una notificacion de un nuevo reclamo de parte de un usuario del viaje que se realizo.</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>Contabilizar votos del reclamo</t>
+  </si>
+  <si>
+    <t>El sistema contabilizara los votos de los pasajeros de un nuevo reclamo y si es de mas del 50% los votos a favor se verificara como valido el reclamo.</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>Enviar notificacion del estado del reclamo</t>
+  </si>
+  <si>
+    <t>El sistema enviara una notificacion al usuario si su reclamo ha sido aprobado o no.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -82,13 +136,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -316,8 +363,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,17 +393,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -365,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,20 +420,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -413,6 +459,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -750,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,18 +809,18 @@
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
-    <col min="6" max="6" width="50.85546875" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -783,77 +832,127 @@
     </row>
     <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
+      <c r="B8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="8"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -861,7 +960,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -869,7 +968,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
@@ -877,7 +976,7 @@
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
@@ -885,7 +984,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
@@ -893,7 +992,7 @@
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
@@ -901,7 +1000,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -909,7 +1008,7 @@
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -917,7 +1016,7 @@
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -925,7 +1024,7 @@
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="15"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -933,7 +1032,7 @@
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
@@ -941,7 +1040,7 @@
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="15"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
@@ -949,7 +1048,7 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -957,7 +1056,7 @@
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:F3"/>
@@ -965,6 +1064,7 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -984,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1002,14 +1102,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1024,63 +1124,63 @@
     </row>
     <row r="3" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="5"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="31"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="32"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="33"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1089,9 +1189,9 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1100,9 +1200,9 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1111,9 +1211,9 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1123,41 +1223,41 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1168,7 +1268,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="19"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -1179,7 +1279,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -1190,7 +1290,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -1201,7 +1301,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1212,7 +1312,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="19"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -1223,7 +1323,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="19"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -1234,7 +1334,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="19"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1245,7 +1345,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="19"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1256,7 +1356,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1267,7 +1367,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Agregada la matriz de incidencia
</commit_message>
<xml_diff>
--- a/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
+++ b/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
-    <sheet name="MATRIZ" sheetId="5" r:id="rId2"/>
+    <sheet name="MATRIZ DE INCIDENCIA" sheetId="5" r:id="rId2"/>
     <sheet name="ITERACION2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -342,13 +342,22 @@
   </si>
   <si>
     <t>El sistema debe permitir acceso a determinadas funciones según el tipo de usuario que inicie sesión</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>Duplicidad</t>
+  </si>
+  <si>
+    <t>Conflicto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -400,8 +409,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,8 +434,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7E1CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -594,13 +627,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -693,6 +806,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1030,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1603,13 +1749,2150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="31" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+    </row>
+    <row r="2" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="41"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z2" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="41"/>
+      <c r="B3" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42">
+        <v>1</v>
+      </c>
+      <c r="E3" s="42">
+        <v>1</v>
+      </c>
+      <c r="F3" s="42">
+        <v>1</v>
+      </c>
+      <c r="G3" s="42">
+        <v>1</v>
+      </c>
+      <c r="H3" s="42">
+        <v>1</v>
+      </c>
+      <c r="I3" s="42">
+        <v>1</v>
+      </c>
+      <c r="J3" s="42">
+        <v>1</v>
+      </c>
+      <c r="K3" s="42">
+        <v>1</v>
+      </c>
+      <c r="L3" s="42">
+        <v>1</v>
+      </c>
+      <c r="M3" s="42">
+        <v>1</v>
+      </c>
+      <c r="N3" s="42">
+        <v>1</v>
+      </c>
+      <c r="O3" s="42">
+        <v>1</v>
+      </c>
+      <c r="P3" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="42">
+        <v>1</v>
+      </c>
+      <c r="R3" s="42">
+        <v>1</v>
+      </c>
+      <c r="S3" s="42">
+        <v>1</v>
+      </c>
+      <c r="T3" s="42">
+        <v>1</v>
+      </c>
+      <c r="U3" s="42">
+        <v>1</v>
+      </c>
+      <c r="V3" s="42">
+        <v>1</v>
+      </c>
+      <c r="W3" s="42">
+        <v>1</v>
+      </c>
+      <c r="X3" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="41"/>
+      <c r="B4" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42">
+        <v>1</v>
+      </c>
+      <c r="F4" s="42">
+        <v>1</v>
+      </c>
+      <c r="G4" s="42">
+        <v>1</v>
+      </c>
+      <c r="H4" s="42">
+        <v>1</v>
+      </c>
+      <c r="I4" s="42">
+        <v>1</v>
+      </c>
+      <c r="J4" s="42">
+        <v>1</v>
+      </c>
+      <c r="K4" s="42">
+        <v>1</v>
+      </c>
+      <c r="L4" s="42">
+        <v>1</v>
+      </c>
+      <c r="M4" s="42">
+        <v>1</v>
+      </c>
+      <c r="N4" s="42">
+        <v>1</v>
+      </c>
+      <c r="O4" s="42">
+        <v>1</v>
+      </c>
+      <c r="P4" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="42">
+        <v>1</v>
+      </c>
+      <c r="R4" s="42">
+        <v>1</v>
+      </c>
+      <c r="S4" s="42">
+        <v>1</v>
+      </c>
+      <c r="T4" s="42">
+        <v>1</v>
+      </c>
+      <c r="U4" s="42">
+        <v>1</v>
+      </c>
+      <c r="V4" s="42">
+        <v>1</v>
+      </c>
+      <c r="W4" s="42">
+        <v>1</v>
+      </c>
+      <c r="X4" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="41"/>
+      <c r="B5" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42">
+        <v>1</v>
+      </c>
+      <c r="G5" s="42">
+        <v>1</v>
+      </c>
+      <c r="H5" s="42">
+        <v>1</v>
+      </c>
+      <c r="I5" s="42">
+        <v>1</v>
+      </c>
+      <c r="J5" s="42">
+        <v>1</v>
+      </c>
+      <c r="K5" s="42">
+        <v>1</v>
+      </c>
+      <c r="L5" s="42">
+        <v>1</v>
+      </c>
+      <c r="M5" s="42">
+        <v>1</v>
+      </c>
+      <c r="N5" s="42">
+        <v>1</v>
+      </c>
+      <c r="O5" s="42">
+        <v>1</v>
+      </c>
+      <c r="P5" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="42">
+        <v>1</v>
+      </c>
+      <c r="R5" s="42">
+        <v>1</v>
+      </c>
+      <c r="S5" s="42">
+        <v>1</v>
+      </c>
+      <c r="T5" s="42">
+        <v>1</v>
+      </c>
+      <c r="U5" s="42">
+        <v>1</v>
+      </c>
+      <c r="V5" s="42">
+        <v>1</v>
+      </c>
+      <c r="W5" s="42">
+        <v>1</v>
+      </c>
+      <c r="X5" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="41"/>
+      <c r="B6" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="43">
+        <v>2</v>
+      </c>
+      <c r="H6" s="42">
+        <v>1</v>
+      </c>
+      <c r="I6" s="42">
+        <v>1</v>
+      </c>
+      <c r="J6" s="42">
+        <v>1</v>
+      </c>
+      <c r="K6" s="42">
+        <v>1</v>
+      </c>
+      <c r="L6" s="42">
+        <v>1</v>
+      </c>
+      <c r="M6" s="42">
+        <v>1</v>
+      </c>
+      <c r="N6" s="42">
+        <v>1</v>
+      </c>
+      <c r="O6" s="42">
+        <v>1</v>
+      </c>
+      <c r="P6" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="42">
+        <v>1</v>
+      </c>
+      <c r="R6" s="42">
+        <v>1</v>
+      </c>
+      <c r="S6" s="42">
+        <v>1</v>
+      </c>
+      <c r="T6" s="42">
+        <v>1</v>
+      </c>
+      <c r="U6" s="42">
+        <v>1</v>
+      </c>
+      <c r="V6" s="42">
+        <v>1</v>
+      </c>
+      <c r="W6" s="42">
+        <v>1</v>
+      </c>
+      <c r="X6" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="41"/>
+      <c r="B7" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42">
+        <v>1</v>
+      </c>
+      <c r="I7" s="42">
+        <v>1</v>
+      </c>
+      <c r="J7" s="42">
+        <v>1</v>
+      </c>
+      <c r="K7" s="42">
+        <v>1</v>
+      </c>
+      <c r="L7" s="42">
+        <v>1</v>
+      </c>
+      <c r="M7" s="42">
+        <v>1</v>
+      </c>
+      <c r="N7" s="42">
+        <v>1</v>
+      </c>
+      <c r="O7" s="42">
+        <v>1</v>
+      </c>
+      <c r="P7" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="42">
+        <v>1</v>
+      </c>
+      <c r="R7" s="43">
+        <v>2</v>
+      </c>
+      <c r="S7" s="42">
+        <v>1</v>
+      </c>
+      <c r="T7" s="42">
+        <v>1</v>
+      </c>
+      <c r="U7" s="42">
+        <v>1</v>
+      </c>
+      <c r="V7" s="42">
+        <v>1</v>
+      </c>
+      <c r="W7" s="42">
+        <v>1</v>
+      </c>
+      <c r="X7" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="41"/>
+      <c r="B8" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42">
+        <v>1</v>
+      </c>
+      <c r="J8" s="42">
+        <v>1</v>
+      </c>
+      <c r="K8" s="42">
+        <v>1</v>
+      </c>
+      <c r="L8" s="42">
+        <v>1</v>
+      </c>
+      <c r="M8" s="42">
+        <v>1</v>
+      </c>
+      <c r="N8" s="42">
+        <v>1</v>
+      </c>
+      <c r="O8" s="42">
+        <v>1</v>
+      </c>
+      <c r="P8" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="42">
+        <v>1</v>
+      </c>
+      <c r="R8" s="42">
+        <v>1</v>
+      </c>
+      <c r="S8" s="42">
+        <v>1</v>
+      </c>
+      <c r="T8" s="42">
+        <v>1</v>
+      </c>
+      <c r="U8" s="42">
+        <v>1</v>
+      </c>
+      <c r="V8" s="42">
+        <v>1</v>
+      </c>
+      <c r="W8" s="42">
+        <v>1</v>
+      </c>
+      <c r="X8" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="41"/>
+      <c r="B9" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42">
+        <v>1</v>
+      </c>
+      <c r="K9" s="42">
+        <v>1</v>
+      </c>
+      <c r="L9" s="42">
+        <v>1</v>
+      </c>
+      <c r="M9" s="42">
+        <v>1</v>
+      </c>
+      <c r="N9" s="42">
+        <v>1</v>
+      </c>
+      <c r="O9" s="42">
+        <v>1</v>
+      </c>
+      <c r="P9" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>1</v>
+      </c>
+      <c r="R9" s="42">
+        <v>1</v>
+      </c>
+      <c r="S9" s="42">
+        <v>1</v>
+      </c>
+      <c r="T9" s="42">
+        <v>1</v>
+      </c>
+      <c r="U9" s="42">
+        <v>1</v>
+      </c>
+      <c r="V9" s="42">
+        <v>1</v>
+      </c>
+      <c r="W9" s="42">
+        <v>1</v>
+      </c>
+      <c r="X9" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
+      <c r="B10" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="42">
+        <v>1</v>
+      </c>
+      <c r="L10" s="42">
+        <v>1</v>
+      </c>
+      <c r="M10" s="42">
+        <v>1</v>
+      </c>
+      <c r="N10" s="42">
+        <v>1</v>
+      </c>
+      <c r="O10" s="42">
+        <v>1</v>
+      </c>
+      <c r="P10" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="42">
+        <v>1</v>
+      </c>
+      <c r="R10" s="42">
+        <v>1</v>
+      </c>
+      <c r="S10" s="42">
+        <v>1</v>
+      </c>
+      <c r="T10" s="42">
+        <v>1</v>
+      </c>
+      <c r="U10" s="42">
+        <v>1</v>
+      </c>
+      <c r="V10" s="42">
+        <v>1</v>
+      </c>
+      <c r="W10" s="42">
+        <v>1</v>
+      </c>
+      <c r="X10" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="41"/>
+      <c r="B11" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42">
+        <v>1</v>
+      </c>
+      <c r="M11" s="42">
+        <v>1</v>
+      </c>
+      <c r="N11" s="42">
+        <v>1</v>
+      </c>
+      <c r="O11" s="42">
+        <v>1</v>
+      </c>
+      <c r="P11" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="42">
+        <v>1</v>
+      </c>
+      <c r="R11" s="42">
+        <v>1</v>
+      </c>
+      <c r="S11" s="42">
+        <v>1</v>
+      </c>
+      <c r="T11" s="42">
+        <v>1</v>
+      </c>
+      <c r="U11" s="42">
+        <v>1</v>
+      </c>
+      <c r="V11" s="42">
+        <v>1</v>
+      </c>
+      <c r="W11" s="42">
+        <v>1</v>
+      </c>
+      <c r="X11" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="41"/>
+      <c r="B12" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="42">
+        <v>1</v>
+      </c>
+      <c r="N12" s="42">
+        <v>1</v>
+      </c>
+      <c r="O12" s="42">
+        <v>1</v>
+      </c>
+      <c r="P12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="42">
+        <v>1</v>
+      </c>
+      <c r="R12" s="42">
+        <v>1</v>
+      </c>
+      <c r="S12" s="42">
+        <v>1</v>
+      </c>
+      <c r="T12" s="42">
+        <v>1</v>
+      </c>
+      <c r="U12" s="42">
+        <v>1</v>
+      </c>
+      <c r="V12" s="42">
+        <v>1</v>
+      </c>
+      <c r="W12" s="42">
+        <v>1</v>
+      </c>
+      <c r="X12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="41"/>
+      <c r="B13" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="42">
+        <v>1</v>
+      </c>
+      <c r="O13" s="42">
+        <v>1</v>
+      </c>
+      <c r="P13" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="42">
+        <v>1</v>
+      </c>
+      <c r="R13" s="42">
+        <v>1</v>
+      </c>
+      <c r="S13" s="42">
+        <v>1</v>
+      </c>
+      <c r="T13" s="42">
+        <v>1</v>
+      </c>
+      <c r="U13" s="42">
+        <v>1</v>
+      </c>
+      <c r="V13" s="42">
+        <v>1</v>
+      </c>
+      <c r="W13" s="42">
+        <v>1</v>
+      </c>
+      <c r="X13" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A14" s="41"/>
+      <c r="B14" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42">
+        <v>1</v>
+      </c>
+      <c r="P14" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>1</v>
+      </c>
+      <c r="R14" s="42">
+        <v>1</v>
+      </c>
+      <c r="S14" s="42">
+        <v>1</v>
+      </c>
+      <c r="T14" s="42">
+        <v>1</v>
+      </c>
+      <c r="U14" s="42">
+        <v>1</v>
+      </c>
+      <c r="V14" s="42">
+        <v>1</v>
+      </c>
+      <c r="W14" s="42">
+        <v>1</v>
+      </c>
+      <c r="X14" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="41"/>
+      <c r="B15" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="42">
+        <v>1</v>
+      </c>
+      <c r="R15" s="42">
+        <v>1</v>
+      </c>
+      <c r="S15" s="42">
+        <v>1</v>
+      </c>
+      <c r="T15" s="42">
+        <v>1</v>
+      </c>
+      <c r="U15" s="42">
+        <v>1</v>
+      </c>
+      <c r="V15" s="42">
+        <v>1</v>
+      </c>
+      <c r="W15" s="42">
+        <v>1</v>
+      </c>
+      <c r="X15" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16" s="41"/>
+      <c r="B16" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="42">
+        <v>1</v>
+      </c>
+      <c r="R16" s="42">
+        <v>1</v>
+      </c>
+      <c r="S16" s="42">
+        <v>1</v>
+      </c>
+      <c r="T16" s="42">
+        <v>1</v>
+      </c>
+      <c r="U16" s="42">
+        <v>1</v>
+      </c>
+      <c r="V16" s="42">
+        <v>1</v>
+      </c>
+      <c r="W16" s="42">
+        <v>1</v>
+      </c>
+      <c r="X16" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A17" s="41"/>
+      <c r="B17" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="42">
+        <v>1</v>
+      </c>
+      <c r="S17" s="42">
+        <v>1</v>
+      </c>
+      <c r="T17" s="42">
+        <v>1</v>
+      </c>
+      <c r="U17" s="42">
+        <v>1</v>
+      </c>
+      <c r="V17" s="42">
+        <v>1</v>
+      </c>
+      <c r="W17" s="42">
+        <v>1</v>
+      </c>
+      <c r="X17" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="41"/>
+      <c r="B18" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="42">
+        <v>1</v>
+      </c>
+      <c r="T18" s="42">
+        <v>1</v>
+      </c>
+      <c r="U18" s="42">
+        <v>1</v>
+      </c>
+      <c r="V18" s="42">
+        <v>1</v>
+      </c>
+      <c r="W18" s="42">
+        <v>1</v>
+      </c>
+      <c r="X18" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="41"/>
+      <c r="B19" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="42">
+        <v>1</v>
+      </c>
+      <c r="U19" s="42">
+        <v>1</v>
+      </c>
+      <c r="V19" s="42">
+        <v>1</v>
+      </c>
+      <c r="W19" s="42">
+        <v>1</v>
+      </c>
+      <c r="X19" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20" s="41"/>
+      <c r="B20" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="42">
+        <v>1</v>
+      </c>
+      <c r="V20" s="42">
+        <v>1</v>
+      </c>
+      <c r="W20" s="42">
+        <v>1</v>
+      </c>
+      <c r="X20" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="41"/>
+      <c r="B21" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="42">
+        <v>1</v>
+      </c>
+      <c r="W21" s="42">
+        <v>1</v>
+      </c>
+      <c r="X21" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="41"/>
+      <c r="B22" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42">
+        <v>1</v>
+      </c>
+      <c r="X22" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="41"/>
+      <c r="B23" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="41"/>
+      <c r="B24" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="41"/>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25" s="41"/>
+      <c r="B25" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="42">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26" s="41"/>
+      <c r="B26" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
+      <c r="U26" s="41"/>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="42">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A27" s="41"/>
+      <c r="B27" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="41"/>
+      <c r="AB27" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A28" s="41"/>
+      <c r="B28" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41"/>
+      <c r="Z28" s="41"/>
+      <c r="AA28" s="41"/>
+      <c r="AB28" s="41"/>
+      <c r="AC28" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A29" s="41"/>
+      <c r="B29" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="41"/>
+      <c r="AB29" s="41"/>
+      <c r="AC29" s="41"/>
+      <c r="AD29" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A30" s="41"/>
+      <c r="B30" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="41"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="41"/>
+      <c r="AB30" s="41"/>
+      <c r="AC30" s="41"/>
+      <c r="AD30" s="41"/>
+      <c r="AE30" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A31" s="41"/>
+      <c r="B31" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="50"/>
+      <c r="Z31" s="50"/>
+      <c r="AA31" s="50"/>
+      <c r="AB31" s="50"/>
+      <c r="AC31" s="50"/>
+      <c r="AD31" s="50"/>
+      <c r="AE31" s="51"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A32" s="41"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="41"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="41"/>
+      <c r="Y32" s="41"/>
+      <c r="Z32" s="41"/>
+      <c r="AA32" s="41"/>
+      <c r="AB32" s="41"/>
+      <c r="AC32" s="41"/>
+      <c r="AD32" s="41"/>
+      <c r="AE32" s="41"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A33" s="41"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="41"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="41"/>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="41"/>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="41"/>
+      <c r="AD33" s="41"/>
+      <c r="AE33" s="41"/>
+    </row>
+    <row r="34" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="42">
+        <v>1</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="41"/>
+      <c r="V34" s="41"/>
+      <c r="W34" s="41"/>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="41"/>
+      <c r="Z34" s="41"/>
+      <c r="AA34" s="41"/>
+      <c r="AB34" s="41"/>
+      <c r="AC34" s="41"/>
+      <c r="AD34" s="41"/>
+      <c r="AE34" s="41"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A35" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="42">
+        <v>2</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="41"/>
+      <c r="V35" s="41"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="41"/>
+      <c r="Y35" s="41"/>
+      <c r="Z35" s="41"/>
+      <c r="AA35" s="41"/>
+      <c r="AB35" s="41"/>
+      <c r="AC35" s="41"/>
+      <c r="AD35" s="41"/>
+      <c r="AE35" s="41"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A36" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="42">
+        <v>3</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
+      <c r="V36" s="41"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="41"/>
+      <c r="Y36" s="41"/>
+      <c r="Z36" s="41"/>
+      <c r="AA36" s="41"/>
+      <c r="AB36" s="41"/>
+      <c r="AC36" s="41"/>
+      <c r="AD36" s="41"/>
+      <c r="AE36" s="41"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add CU Chat en tiempo real - Iteracion2
</commit_message>
<xml_diff>
--- a/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
+++ b/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mis Documentos\GitHub\ElmerX\Desarrollo\STSM\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Documents\GCM\ElmerX\Desarrollo\STSM\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22F6CF2-981B-43A5-BEE8-B2F261F40E83}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -222,12 +223,15 @@
   </si>
   <si>
     <t>El sistema mostrará mensajes predeterminados para poder ser de fácil acceso y rápido envío.</t>
+  </si>
+  <si>
+    <t>CU Chat en tiempo real</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -300,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -474,13 +478,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -577,10 +594,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
-    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -608,7 +646,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -625,7 +663,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,6 +738,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -735,6 +790,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -910,14 +982,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
@@ -1178,7 +1250,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="28" t="s">
         <v>57</v>
@@ -1318,7 +1390,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:F3"/>
+  <autoFilter ref="B3:F3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
@@ -1328,26 +1400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
@@ -1359,7 +1431,7 @@
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="29" t="s">
         <v>0</v>
@@ -1371,7 +1443,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1381,7 +1453,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="16" t="s">
         <v>1</v>
@@ -1408,7 +1480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="34"/>
@@ -1419,7 +1491,7 @@
       <c r="H4" s="39"/>
       <c r="I4" s="31"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
       <c r="C5" s="35"/>
@@ -1430,7 +1502,7 @@
       <c r="H5" s="40"/>
       <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="35"/>
@@ -1441,7 +1513,7 @@
       <c r="H6" s="41"/>
       <c r="I6" s="33"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="8"/>
       <c r="C7" s="5"/>
@@ -1452,7 +1524,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
@@ -1463,7 +1535,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
@@ -1474,7 +1546,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1485,7 +1557,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
@@ -1496,7 +1568,7 @@
       <c r="H11" s="24"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="27"/>
       <c r="C12" s="23"/>
@@ -1507,7 +1579,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:9" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
@@ -1518,7 +1590,7 @@
       <c r="H13" s="24"/>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1529,7 +1601,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
@@ -1540,7 +1612,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1551,7 +1623,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
@@ -1562,7 +1634,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1570,66 +1642,143 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="18"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="43">
+        <v>9</v>
+      </c>
+      <c r="I19" s="46"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="47"/>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="47"/>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="18"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="47"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="18"/>
+      <c r="B23" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="47"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="G19:G24"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="I19:I24"/>
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="C4:C6"/>
@@ -1638,5 +1787,6 @@
     <mergeCell ref="H4:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadiendo 2 estados y 2 auditoria
</commit_message>
<xml_diff>
--- a/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
+++ b/Desarrollo/STSM/Requisitos/STSM_LR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diaz\Documents\gestion\ElmerX\Desarrollo\STSM\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB85CF8-9A88-4DA8-9968-5DDBBA754AD0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B810CAF-110C-4631-9BD4-A91E6C521853}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="126">
   <si>
     <t>LISTA DE REQUISITOS DEL SISTEMA XYZ</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>CU Chat en tiempo real</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ver la información del viaje: la ruta, numero de asientos disponibles, información del automovil (placa, modelo, numero de asientos, color, SOAT).</t>
   </si>
 </sst>
 </file>
@@ -870,6 +873,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -889,15 +901,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4030,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22:I27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4115,7 +4118,7 @@
       <c r="G4" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="42">
         <v>1</v>
       </c>
       <c r="I4" s="57"/>
@@ -4180,10 +4183,10 @@
         <v>33</v>
       </c>
       <c r="G7" s="54"/>
-      <c r="H7" s="49"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="59"/>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="28" t="s">
         <v>85</v>
@@ -4198,12 +4201,12 @@
         <v>86</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="48">
+      <c r="H8" s="42">
         <v>1</v>
       </c>
       <c r="I8" s="60"/>
@@ -4225,8 +4228,8 @@
       <c r="F9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="61"/>
     </row>
     <row r="10" spans="1:9" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4384,13 +4387,13 @@
       <c r="F16" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="42">
         <v>5</v>
       </c>
-      <c r="I16" s="48"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -4409,9 +4412,9 @@
       <c r="F17" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -4430,13 +4433,13 @@
       <c r="F18" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="42">
         <v>4</v>
       </c>
-      <c r="I18" s="48"/>
+      <c r="I18" s="42"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -4455,9 +4458,9 @@
       <c r="F19" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
       <c r="J19" s="51"/>
     </row>
     <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4477,13 +4480,13 @@
       <c r="F20" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="42">
         <v>6</v>
       </c>
-      <c r="I20" s="48"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="51"/>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4503,9 +4506,9 @@
       <c r="F21" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
       <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:10" s="35" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4524,13 +4527,13 @@
       <c r="F22" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="50" t="s">
+      <c r="G22" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="41">
         <v>9</v>
       </c>
-      <c r="I22" s="45"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="34"/>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4549,9 +4552,9 @@
       <c r="F23" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="46"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="49"/>
       <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4570,9 +4573,9 @@
       <c r="F24" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="46"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="49"/>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
@@ -4590,9 +4593,9 @@
       <c r="F25" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="46"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="49"/>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
@@ -4610,9 +4613,9 @@
       <c r="F26" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="46"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="49"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
@@ -4630,9 +4633,9 @@
       <c r="F27" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="47"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="50"/>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -4651,13 +4654,13 @@
       <c r="F28" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="H28" s="41">
-        <v>1</v>
-      </c>
-      <c r="I28" s="42"/>
+      <c r="H28" s="44">
+        <v>1</v>
+      </c>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="B29" s="31" t="s">
@@ -4675,9 +4678,9 @@
       <c r="F29" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="50"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="43"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="B30" s="31" t="s">
@@ -4695,13 +4698,13 @@
       <c r="F30" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="H30" s="41">
-        <v>1</v>
-      </c>
-      <c r="I30" s="42"/>
+      <c r="H30" s="44">
+        <v>1</v>
+      </c>
+      <c r="I30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B31" s="31" t="s">
@@ -4719,9 +4722,9 @@
       <c r="F31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="50"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="44"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B32" s="31" t="s">
@@ -4739,9 +4742,9 @@
       <c r="F32" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="50"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="43"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="32">

</xml_diff>